<commit_message>
cambios en el excel sprint
</commit_message>
<xml_diff>
--- a/Planificación/planificacion de la iteracion-Checkface G11.xlsx
+++ b/Planificación/planificacion de la iteracion-Checkface G11.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlik3\Desktop\5to ciclo\Calidad de Software\Proyecto\Checkface\Planificación\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01D92D5-B69D-435A-8141-27EAC803CAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\.m"/>
@@ -335,41 +336,22 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -385,6 +367,15 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -394,17 +385,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -720,11 +721,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -736,451 +737,463 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8">
+      <c r="A2" s="29"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="3">
         <v>44354</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="13">
+      <c r="A4" s="4">
         <v>44197</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="15" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="16">
+      <c r="A5" s="6">
         <v>44228</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="18" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="7">
         <v>2</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="16">
+      <c r="A6" s="6">
         <v>44256</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="18" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="16">
+      <c r="A7" s="6">
         <v>44287</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="18" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="16">
+      <c r="A8" s="6">
         <v>44317</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="18" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="7">
         <v>1</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6">
+        <v>44348</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="6">
+        <v>44378</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6">
+        <v>44409</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="7">
+        <v>3</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="29"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>44368</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4">
+        <v>44198</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="16">
-        <v>44348</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="18" t="s">
+    <row r="18" spans="1:8">
+      <c r="A18" s="6">
+        <v>44229</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="6">
+        <v>44257</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="6">
+        <v>44288</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="6">
+        <v>44318</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="6">
+        <v>44349</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H22" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="16">
-        <v>44378</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="18" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23" s="11">
+        <v>44379</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G23" s="12">
         <v>2</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H23" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="16">
-        <v>44409</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="18" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" s="13">
+        <v>44410</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G24" s="14">
         <v>3</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8">
-        <v>2</v>
-      </c>
-      <c r="G15" s="9">
-        <v>44368</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="13">
-        <v>44198</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="15">
-        <v>1</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="16">
-        <v>44229</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="16">
-        <v>44257</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="18">
-        <v>1</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="16">
-        <v>44288</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="18">
-        <v>1</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="16">
-        <v>44318</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="18">
-        <v>1</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="16">
-        <v>44349</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="18">
-        <v>2</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="22">
-        <v>44379</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="26">
-        <v>2</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="27">
-        <v>44410</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="30">
-        <v>3</v>
-      </c>
-      <c r="H24" s="30" t="s">
+      <c r="H24" s="14" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A14:E15"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B17:E17"/>
@@ -1189,18 +1202,6 @@
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="A14:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>